<commit_message>
Cambios al excel con los datos mejor organizados
</commit_message>
<xml_diff>
--- a/src/Entrega2.xlsx
+++ b/src/Entrega2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicoh\OneDrive\Documentos\UBA\1ero 2020\Numerico\TPs\entrega-2\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48041B45-3DCB-431B-80FF-A8DCB5E11575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D84CD10-F7C4-4FCA-AB10-6E8AA117E11C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{018AF0C9-1332-47C6-90FC-A18FAE2476D2}"/>
   </bookViews>
@@ -424,7 +424,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -443,6 +443,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -456,12 +462,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1110,10 +1117,10 @@
                   <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>103</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>410</c:v>
+                  <c:v>257</c:v>
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>286</c:v>
@@ -1179,13 +1186,13 @@
                   <c:v>2599</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>4376</c:v>
+                  <c:v>5605</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>7578</c:v>
+                  <c:v>5605</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>4861</c:v>
+                  <c:v>5605</c:v>
                 </c:pt>
                 <c:pt idx="94">
                   <c:v>2116</c:v>
@@ -1230,16 +1237,16 @@
                   <c:v>2633</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>2641</c:v>
+                  <c:v>1523</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>405</c:v>
+                  <c:v>1523</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>2569</c:v>
+                  <c:v>1677</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>785</c:v>
+                  <c:v>1677</c:v>
                 </c:pt>
                 <c:pt idx="112">
                   <c:v>2051</c:v>
@@ -2152,7 +2159,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="20" name="Chart 1">
+        <xdr:cNvPr id="20" name="Tabla">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{721B9782-D9FB-423E-B211-D6FFA1D641F9}"/>
@@ -2475,8 +2482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CD16D5C-3915-4797-AD42-A46A7196562F}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N104" sqref="N104"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3656,10 +3663,12 @@
         <v>69</v>
       </c>
       <c r="E69" s="1">
+        <v>256</v>
+      </c>
+      <c r="F69" s="2">
         <v>103</v>
       </c>
-      <c r="F69" s="2"/>
-      <c r="G69" s="3"/>
+      <c r="G69" s="5"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
@@ -3675,10 +3684,12 @@
         <v>70</v>
       </c>
       <c r="E70" s="1">
+        <v>257</v>
+      </c>
+      <c r="F70" s="2">
         <v>410</v>
       </c>
-      <c r="F70" s="2"/>
-      <c r="G70" s="3"/>
+      <c r="G70" s="5"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
@@ -3696,7 +3707,7 @@
       <c r="E71" s="1">
         <v>286</v>
       </c>
-      <c r="G71" s="3"/>
+      <c r="G71" s="5"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
@@ -4052,9 +4063,11 @@
         <v>92</v>
       </c>
       <c r="E92" s="1">
+        <v>5605</v>
+      </c>
+      <c r="F92" s="3">
         <v>4376</v>
       </c>
-      <c r="F92" s="3"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
@@ -4070,9 +4083,11 @@
         <v>93</v>
       </c>
       <c r="E93" s="1">
+        <v>5605</v>
+      </c>
+      <c r="F93" s="3">
         <v>7578</v>
       </c>
-      <c r="F93" s="3"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
@@ -4088,9 +4103,11 @@
         <v>94</v>
       </c>
       <c r="E94" s="1">
+        <v>5605</v>
+      </c>
+      <c r="F94" s="3">
         <v>4861</v>
       </c>
-      <c r="F94" s="3"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
@@ -4344,9 +4361,11 @@
         <v>109</v>
       </c>
       <c r="E109" s="1">
+        <v>1523</v>
+      </c>
+      <c r="F109" s="3">
         <v>2641</v>
       </c>
-      <c r="F109" s="3"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
@@ -4362,9 +4381,11 @@
         <v>110</v>
       </c>
       <c r="E110" s="1">
+        <v>1523</v>
+      </c>
+      <c r="F110" s="3">
         <v>405</v>
       </c>
-      <c r="F110" s="3"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
@@ -4380,9 +4401,11 @@
         <v>111</v>
       </c>
       <c r="E111" s="1">
+        <v>1677</v>
+      </c>
+      <c r="F111" s="4">
         <v>2569</v>
       </c>
-      <c r="F111" s="4"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
@@ -4398,9 +4421,11 @@
         <v>112</v>
       </c>
       <c r="E112" s="1">
+        <v>1677</v>
+      </c>
+      <c r="F112" s="4">
         <v>785</v>
       </c>
-      <c r="F112" s="4"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">

</xml_diff>

<commit_message>
Todos los 0 los cambiamos a 1
</commit_message>
<xml_diff>
--- a/src/Entrega2.xlsx
+++ b/src/Entrega2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicoh\OneDrive\Documentos\UBA\1ero 2020\Numerico\TPs\entrega-2\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D84CD10-F7C4-4FCA-AB10-6E8AA117E11C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95673FD-B2D6-4CC4-BD9A-A32E8222AC3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{018AF0C9-1332-47C6-90FC-A18FAE2476D2}"/>
   </bookViews>
@@ -913,91 +913,91 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1048576"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>1</c:v>
@@ -1009,79 +1009,79 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>2</c:v>
@@ -2482,8 +2482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CD16D5C-3915-4797-AD42-A46A7196562F}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F113" sqref="F113"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49:E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2507,7 +2507,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2524,7 +2524,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2541,7 +2541,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -2558,7 +2558,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -2575,7 +2575,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -2592,7 +2592,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -2609,7 +2609,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -2626,7 +2626,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -2643,7 +2643,7 @@
         <v>9</v>
       </c>
       <c r="E9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -2660,7 +2660,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -2677,7 +2677,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2694,7 +2694,7 @@
         <v>12</v>
       </c>
       <c r="E12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2711,7 +2711,7 @@
         <v>13</v>
       </c>
       <c r="E13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -2728,7 +2728,7 @@
         <v>14</v>
       </c>
       <c r="E14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -2745,7 +2745,7 @@
         <v>15</v>
       </c>
       <c r="E15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2762,7 +2762,7 @@
         <v>16</v>
       </c>
       <c r="E16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -2779,7 +2779,7 @@
         <v>17</v>
       </c>
       <c r="E17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -2796,7 +2796,7 @@
         <v>18</v>
       </c>
       <c r="E18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -2813,7 +2813,7 @@
         <v>19</v>
       </c>
       <c r="E19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -2830,7 +2830,7 @@
         <v>20</v>
       </c>
       <c r="E20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -2847,7 +2847,7 @@
         <v>21</v>
       </c>
       <c r="E21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -2864,7 +2864,7 @@
         <v>22</v>
       </c>
       <c r="E22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -2881,7 +2881,7 @@
         <v>23</v>
       </c>
       <c r="E23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -2898,7 +2898,7 @@
         <v>24</v>
       </c>
       <c r="E24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -2915,7 +2915,7 @@
         <v>25</v>
       </c>
       <c r="E25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -2949,7 +2949,7 @@
         <v>27</v>
       </c>
       <c r="E27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -2966,7 +2966,7 @@
         <v>28</v>
       </c>
       <c r="E28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -2983,7 +2983,7 @@
         <v>29</v>
       </c>
       <c r="E29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -3051,7 +3051,7 @@
         <v>33</v>
       </c>
       <c r="E33" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -3068,7 +3068,7 @@
         <v>34</v>
       </c>
       <c r="E34" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -3085,7 +3085,7 @@
         <v>35</v>
       </c>
       <c r="E35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -3102,7 +3102,7 @@
         <v>36</v>
       </c>
       <c r="E36" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -3119,7 +3119,7 @@
         <v>37</v>
       </c>
       <c r="E37" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -3136,7 +3136,7 @@
         <v>38</v>
       </c>
       <c r="E38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -3153,7 +3153,7 @@
         <v>39</v>
       </c>
       <c r="E39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -3187,7 +3187,7 @@
         <v>41</v>
       </c>
       <c r="E41" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -3204,7 +3204,7 @@
         <v>42</v>
       </c>
       <c r="E42" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -3221,7 +3221,7 @@
         <v>43</v>
       </c>
       <c r="E43" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -3238,7 +3238,7 @@
         <v>44</v>
       </c>
       <c r="E44" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -3255,7 +3255,7 @@
         <v>45</v>
       </c>
       <c r="E45" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -3272,7 +3272,7 @@
         <v>46</v>
       </c>
       <c r="E46" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -3289,7 +3289,7 @@
         <v>47</v>
       </c>
       <c r="E47" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -3306,7 +3306,7 @@
         <v>48</v>
       </c>
       <c r="E48" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -3340,7 +3340,7 @@
         <v>50</v>
       </c>
       <c r="E50" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -3357,7 +3357,7 @@
         <v>51</v>
       </c>
       <c r="E51" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -3374,7 +3374,7 @@
         <v>52</v>
       </c>
       <c r="E52" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -3391,7 +3391,7 @@
         <v>53</v>
       </c>
       <c r="E53" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -3408,7 +3408,7 @@
         <v>54</v>
       </c>
       <c r="E54" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -3425,7 +3425,7 @@
         <v>55</v>
       </c>
       <c r="E55" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -3442,7 +3442,7 @@
         <v>56</v>
       </c>
       <c r="E56" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -3459,7 +3459,7 @@
         <v>57</v>
       </c>
       <c r="E57" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>